<commit_message>
fixed all I knew bags
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="458">
   <si>
     <t xml:space="preserve">Toifanin nomi</t>
   </si>
@@ -45,7 +45,7 @@
     <t xml:space="preserve">Storm 09</t>
   </si>
   <si>
-    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim Xizmat ko'rsatish zonasi                26kv.m         Inverter                                                 Bor      Asosiy rejimlar                 sovutish va isitish   Energiya sinfi                        A                             Tashqi shovqin darajasi             55.5 dB                         Ichki shovqin darajasi                 36 dB    Sovutgichning turi                       R41OA    Havo oqimining hajmi                   417 m3/s       Ichki blokning vazni                  7.5 kg             Tashqi blokning vazni                  22.8 kg             </t>
+    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim Xizmat ko'rsatish zonasi  26kv.m . Inverter Bor.   Asosiy rejimlar sovutish va isitish   Energiya sinfi A Tashqi shovqin darajasi 55.5 dB Ichki shovqin darajasi 36 dB    Sovutgichning turi R41OA Havo oqimining hajmi 417 m3/s   Ichki blokning vazni 7.5 kg Tashqi blokning vazni 22.8 kg</t>
   </si>
   <si>
     <t xml:space="preserve">file/storm-09.jpg</t>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">Oxygen 09</t>
   </si>
   <si>
-    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zona                 26 kv.m         Inverter                                                 Bor      Asosiy rejimla                 sovutish va isitish      Energiya sinfi                                            A        Sovutish rejimida quvvat sarfi             35 Vt        Isitish rejimida quvvat sarfi             3690 Vt         Ichki blok shovqin darajasi              36.5 dB        Tashqi blok shovqin darajasi           55.5 dB      Sovutgichning turi                           R41OA            Havo  oqimining hajmi                  417 m3/s           Ichki   blokning vazni                        7.5 kg                 Tashqi blokning vazni                     22.8 kg               Avto   restart                                                          Turbo rejim                                                              O'z o'zini tozalash</t>
+    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zona 26 kv.m Inverter Bor Asosiy rejimla sovutish va isitish   Energiya sinf A Sovutish rejimida quvvat sarfi  35 Vt   Isitish rejimida quvvat sarfi 3690 Vt Ichki blok shovqin darajasi  36.5 dB  Tashqi blok shovqin darajasi    55.5 dB Sovutgichning turi R41OA  Havo  oqimining hajmi  417 m3/s Ichki   blokning vazni 7.5 kg Tashqi blokning vazni 22.8 kg Avto restart Turbo rejim O'z o'zini tozalash</t>
   </si>
   <si>
     <t xml:space="preserve">file/oxygen-09.jpg</t>
@@ -63,7 +63,7 @@
     <t xml:space="preserve">Trendi 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi           36 kv.m         Inverter                                            Yo'q      Asosiy rejimlar                   sovutish va isitish      Energiya sinfi                                  A        Sovutish rejimida quvvat sarfi    3590 Vt   Isitish rejimida quvvat sarfi                3690 Vt Ichki blok shovqin darajasi             43 dB        Tashqi blok shovqin darajasi          53 dB      Sovutgichning turi                          R41OA            Havo  oqimining hajmi                90 m3/s           Ichki   blokning vazni                  9 kg                 Tashqi blokning vazni                    28 kg                                                                                                            </t>
+    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi  36 kv.m Inverter Yo'q      Asosiy rejimlar                   sovutish va isitish      Energiya sinfi                                  A        Sovutish rejimida quvvat sarfi    3590 Vt   Isitish rejimida quvvat sarfi  3690 Vt Ichki blok shovqin darajasi             43 dB        Tashqi blok shovqin darajasi          53 dB      Sovutgichning turi   R41OA  Havo  oqimining hajmi     90 m3/s   Ichki   blokning vazni   9 kg   Tashqi blokning vazni 28 kg  </t>
   </si>
   <si>
     <t xml:space="preserve">file/trendi-12.jpg</t>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">Desert 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi           36 kv.m         Inverter                                            Yo'q      Asosiy rejimlar                     sovutish va isitish      Energiya sinfi                                              A        Sovutish rejimida quvvat sarfi        3590 Vt    Isitish rejimida quvvat sarfi            3690 Vt Ichki blok shovqin darajasi          43 dB        Tashqi blok shovqin darajasi        53 dB      Sovutgichning turi                           R41OA            Havo  oqimining hajmi                    590 m3/s           Ichki   blokning vazni                  9 kg                 Tashqi blokning vazni                    28 kg                                                                                                            </t>
+    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi  36 kv.m         Inverter           Yo'q      Asosiy rejimlar sovutish va isitish      Energiya sinfi   A        Sovutish rejimida quvvat sarfi        3590 Vt    Isitish rejimida quvvat sarfi            3690 Vt Ichki blok shovqin darajasi          43 dB        Tashqi blok shovqin darajasi        53 dB   Sovutgichning turi   R41OA  Havo  oqimining hajmi       590 m3/s   Ichki   blokning vazni 9 kg  Tashqi blokning vazni  28 kg    </t>
   </si>
   <si>
     <t xml:space="preserve">file/desert-12.jpg</t>
@@ -81,7 +81,7 @@
     <t xml:space="preserve">Frenzi 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi           36 kv.m         Inverter                                            Yo'q      Asosiy rejimlar                 sovutish va isitish      Energiya sinfi                                  A        Sovutish rejimida quvvat sarfi         3590 Vt    Isitish rejimida quvv                      3690 Vt Ichki blok shovqin darajasi          43 dB       Tashqi blok shovqin darajasi       53 dB      Sovutgichning turi                           R41OA                    Havo  oqimining hajmi                       590 m3/s           Ichki   blokning vazni                 9 kg                 Tashqi blokning vazni                  28 kg                                                                                                            </t>
+    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi  36 kv.m    Inverter  Yo'q  Asosiy rejimlar      sovutish va isitish      Energiya sinfi    A  Sovutish rejimida quvvat sarfi  590 Vt    Isitish rejimida quvv     3690 Vt Ichki blok shovqin darajasi    43 dB       Tashqi blok shovqin darajasi    53 dB      Sovutgichning turi  R41OA   Havo  oqimining hajmi    590 m3/s   Ichki   blokning vazni   9 kg   Tashqi blokning vazni    28 kg  </t>
   </si>
   <si>
     <t xml:space="preserve">file/frenzi-12.jpg</t>
@@ -90,7 +90,7 @@
     <t xml:space="preserve">TurboChill 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi           36 kv.m         Inverter                                            Bor      Asosiy rejimlar                 sovutish va isitish      Energiya sinfi                                  A        Sovutish rejimida quvvat sarfi         3050 Vt Isitish rejimida quvvat sarfi              3250 Vt Ichki blok shovqin darajasi              42 dB       Tashqi blok shovqin darajasi         53 dB      Sovutgichning turi                             R41OA                    Havo  oqimining hajmi                      600  m3/s           Ichki   blokning vazni                      8,50 kg                 Tashqi blokning vazni                  25 kg                                                                                                            </t>
+    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi   36 kv.m  Inverter    Bor      Asosiy rejimlar   sovutish va isitish      Energiya sinfi   A     Sovutish rejimida quvvat sarfi         3050 Vt Isitish rejimida quvvat sarfi  3250 Vt Ichki blok shovqin darajasi   42 dB       Tashqi blok shovqin darajasi         53 dB   Sovutgichning turi  R41OA    Havo  oqimining hajmi     600  m3/s Ichki   blokning vazni    8,50 kg Tashqi blokning vazni  25 kg  </t>
   </si>
   <si>
     <t xml:space="preserve">file/turbochill-12.jpg</t>
@@ -99,7 +99,7 @@
     <t xml:space="preserve">DarkMoon 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi           26 kv.m         Inverter                                            Bor      Asosiy rejimlar                 sovutish va isitish      Energiya sinfi                                  A        Sovutish rejimida quvvat sarfi          3050 Vt Isitish rejimida quvvat sarfi                   3250 Vt Ichki blok shovqin darajasi                 42 dB       Tashqi blok shovqin darajasi               53 dB      Sovutgichning turi                             R41OA                    Havo  oqimining hajmi                     600  m3/s           Ichki   blokning vazni                    8,50 kg                 Tashqi blokning vazni                      25 kg                                                                                                            </t>
+    <t xml:space="preserve">Konditsioner turi  Devorga o'rnatiladigan tizim  Xizmat ko'rsatish zonasi   26 kv.m         Inverter  Bor      Asosiy rejimlar   sovutish va isitish      Energiya sinfi    A        Sovutish rejimida quvvat sarfi          3050 Vt Isitish rejimida quvvat sarfi     3250 Vt Ichki blok shovqin darajasi      42 dB       Tashqi blok shovqin darajasi    53 dB      Sovutgichning turi     R41OA   Havo  oqimining hajmi     600  m3/s           Ichki   blokning vazni    8,50 kg  Tashqi blokning vazni      25 kg  </t>
   </si>
   <si>
     <t xml:space="preserve">file/darkmoon-12.jpg</t>
@@ -528,7 +528,7 @@
     <t xml:space="preserve">file/32ME700.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Gaz plita</t>
+    <t xml:space="preserve">GAZ PLITA</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -543,9 +543,6 @@
     <t xml:space="preserve">file/a02.png</t>
   </si>
   <si>
-    <t xml:space="preserve">GAZ PLITA</t>
-  </si>
-  <si>
     <t xml:space="preserve">A02E</t>
   </si>
   <si>
@@ -849,9 +846,6 @@
     <t xml:space="preserve">file/IM7010S08.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">70 L  </t>
-  </si>
-  <si>
     <t xml:space="preserve">IM7009S03</t>
   </si>
   <si>
@@ -1239,6 +1233,9 @@
     <t xml:space="preserve">VENTILYATOR</t>
   </si>
   <si>
+    <t xml:space="preserve">VENTILYATORS</t>
+  </si>
+  <si>
     <t xml:space="preserve">AIR-13R</t>
   </si>
   <si>
@@ -1246,9 +1243,6 @@
   </si>
   <si>
     <t xml:space="preserve">file/air-13r.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VENTILYATORS</t>
   </si>
   <si>
     <t xml:space="preserve">AIR-33R</t>
@@ -1596,8 +1590,8 @@
   </sheetPr>
   <dimension ref="A1:K265"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B142" activeCellId="0" sqref="B142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C132" activeCellId="0" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1669,7 +1663,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="156" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +1688,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="156" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1734,7 +1728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="156" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1754,7 +1748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="156" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -2676,42 +2670,42 @@
     </row>
     <row r="54" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="E54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="E54" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="E55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,1719 +2713,1719 @@
         <v>167</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="E56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="E57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="E57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="E58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C59" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="E59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="E59" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="E60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="E60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="E61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="E61" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="E62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="E62" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="E63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="E63" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="E64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="E64" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="E65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="E65" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="E66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="E66" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B67" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="E67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="E67" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B68" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C68" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="E68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="E68" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B69" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="E69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="E69" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B70" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="E70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="E70" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="E71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="E71" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B72" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C72" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="E72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="E72" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B73" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="E73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="E73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B74" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="E74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="E74" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B75" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="E75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="E75" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B76" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C76" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="E76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="E76" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B77" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="E77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="E77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B78" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="E78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="E78" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B79" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="E79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="E79" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B80" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="E80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="E80" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B81" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C81" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="E81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="E81" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="E82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="E82" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="C83" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="E83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="E83" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="C84" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="E84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E84" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
+    </row>
+    <row r="85" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B85" s="2" t="s">
+      <c r="D85" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="E85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="E85" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="E86" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="C87" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E87" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="E88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E88" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="D89" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="E89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="E89" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C90" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="E90" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="D91" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="E91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="E91" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C92" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C93" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="E93" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="E95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="E95" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C96" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F96" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="E96" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="E97" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C98" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="E98" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C99" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="E99" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D100" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="E100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E100" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C101" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="E101" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C102" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="E102" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D103" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="E103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="E103" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="E104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="E104" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="D105" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="E105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E105" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C106" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F106" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="E106" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C107" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F107" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E107" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C108" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F108" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="E108" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C109" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F109" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="E109" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C110" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="E110" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C111" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="E111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C112" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="E112" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C113" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F113" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="E113" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C114" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="E114" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C115" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="E115" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B116" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D116" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="E116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="E116" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C117" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="E117" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C118" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="E118" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C119" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="E119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="E119" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C120" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="E120" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C121" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="E121" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B122" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D122" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="E122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="E122" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C123" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="E123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F123" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="E123" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C124" s="2" t="s">
+      <c r="D124" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="E124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F124" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="E124" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D125" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="E125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F125" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E125" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C126" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="E126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F126" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="E126" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C127" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="E127" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C128" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="E128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="E128" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="D129" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="E129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F129" s="2" t="s">
         <v>422</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="E129" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C130" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="E130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F130" s="2" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C131" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="E131" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C132" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="E132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="E132" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="D133" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="E133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F133" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="E133" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C134" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="E134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="E134" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C135" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="E135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F135" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="E135" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C136" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F136" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="E136" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C137" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F137" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="E137" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="73.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C138" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F138" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="E138" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E139" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C140" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F140" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="E140" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C141" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="E141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="E141" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5444,7 +5438,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5467,7 +5461,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>